<commit_message>
Corrección Uno a Varios
</commit_message>
<xml_diff>
--- a/Documentos/Copia de FormaConciliacionv3 -.xlsx
+++ b/Documentos/Copia de FormaConciliacionv3 -.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="84">
   <si>
     <t>CONCILIACION DE EGRESOS</t>
   </si>
@@ -229,9 +229,6 @@
     <t>Nuevo</t>
   </si>
   <si>
-    <t>Interno, Pedido ED, pedido Gas, ST</t>
-  </si>
-  <si>
     <t>1,2 Interno,3 Interno , 5, 6 Interno, 7, 8, 9</t>
   </si>
   <si>
@@ -275,6 +272,12 @@
   </si>
   <si>
     <t>Päsar a tipo 4 y eliminar</t>
+  </si>
+  <si>
+    <t>pedido Gas, ST</t>
+  </si>
+  <si>
+    <t>Interno, Pedido ED</t>
   </si>
 </sst>
 </file>
@@ -307,12 +310,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -335,6 +332,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -348,19 +351,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -644,61 +648,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="40.28515625" customWidth="1"/>
     <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.140625" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="F1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>68</v>
+      <c r="F2" s="5" t="s">
+        <v>67</v>
       </c>
       <c r="G2" t="s">
         <v>38</v>
@@ -723,8 +725,8 @@
       <c r="E3" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>69</v>
+      <c r="F3" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="H3" t="s">
         <v>41</v>
@@ -743,96 +745,96 @@
       <c r="E4" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>70</v>
+      <c r="F4" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>68</v>
+      <c r="F5" s="5" t="s">
+        <v>67</v>
       </c>
       <c r="H5" t="s">
         <v>41</v>
       </c>
       <c r="I5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5" t="s">
+      <c r="C6" s="4"/>
+      <c r="D6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5" t="s">
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+      <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8" t="s">
+      <c r="C7" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>71</v>
+      <c r="F7" s="6" t="s">
+        <v>70</v>
       </c>
       <c r="H7" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2" t="s">
+      <c r="B9" s="1"/>
+      <c r="C9" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>74</v>
+      <c r="E9" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="6">
         <v>1</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="9" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
@@ -840,106 +842,118 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+      <c r="A11" s="6">
         <v>2</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="9" t="s">
         <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+      <c r="A12" s="6">
         <v>3</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="9" t="s">
         <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>76</v>
+        <v>83</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="A13" s="4">
         <v>4</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
+      <c r="A14" s="6">
         <v>5</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="9" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="7" t="s">
-        <v>76</v>
+      <c r="E14" s="6" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
+      <c r="A15" s="6">
         <v>6</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="9" t="s">
         <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
+      <c r="A16" s="6">
         <v>7</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="9" t="s">
         <v>42</v>
       </c>
+      <c r="D16" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="7">
+      <c r="A17" s="6">
         <v>8</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="9" t="s">
         <v>42</v>
       </c>
+      <c r="D17" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
+      <c r="A18" s="6">
         <v>9</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="9" t="s">
         <v>43</v>
+      </c>
+      <c r="D18" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1158,41 +1172,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1211,7 +1225,7 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1219,18 +1233,18 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1256,13 +1270,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" t="s">
         <v>78</v>
       </c>
-      <c r="B1" t="s">
-        <v>79</v>
-      </c>
       <c r="E1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1275,7 +1289,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D3" t="str">
         <f>CONCATENATE("Insert into TipoFormaConciliacion values(",$A$2,",",B3,",'');")</f>
@@ -1287,7 +1301,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" ref="D4:D11" si="0">CONCATENATE("Insert into TipoFormaConciliacion values(",$A$2,",",B4,",'');")</f>
@@ -1299,7 +1313,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
@@ -1311,7 +1325,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1319,7 +1333,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
@@ -1331,7 +1345,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
@@ -1343,7 +1357,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
@@ -1355,7 +1369,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
@@ -1367,7 +1381,7 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
@@ -1384,7 +1398,7 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1392,10 +1406,10 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D14" t="str">
-        <f t="shared" ref="D14:D23" si="1">CONCATENATE("Insert into TipoFormaConciliacion values(",$A$12,",",B14,",'');")</f>
+        <f t="shared" ref="D14:D18" si="1">CONCATENATE("Insert into TipoFormaConciliacion values(",$A$12,",",B14,",'');")</f>
         <v>Insert into TipoFormaConciliacion values(2,2,'');</v>
       </c>
     </row>
@@ -1404,7 +1418,7 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="1"/>
@@ -1416,7 +1430,7 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1424,7 +1438,7 @@
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1432,7 +1446,7 @@
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="1"/>
@@ -1444,7 +1458,7 @@
         <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1452,7 +1466,7 @@
         <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1460,7 +1474,7 @@
         <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1473,7 +1487,7 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D23" t="str">
         <f>CONCATENATE("Insert into TipoFormaConciliacion values(",$A$22,",",B23,",'');")</f>
@@ -1485,10 +1499,10 @@
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D24" t="str">
-        <f t="shared" ref="D24:D31" si="2">CONCATENATE("Insert into TipoFormaConciliacion values(",$A$22,",",B24,",'');")</f>
+        <f t="shared" ref="D24:D28" si="2">CONCATENATE("Insert into TipoFormaConciliacion values(",$A$22,",",B24,",'');")</f>
         <v>Insert into TipoFormaConciliacion values(3,2,'');</v>
       </c>
     </row>
@@ -1497,7 +1511,7 @@
         <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="2"/>
@@ -1509,7 +1523,7 @@
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1517,7 +1531,7 @@
         <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="2"/>
@@ -1529,7 +1543,7 @@
         <v>6</v>
       </c>
       <c r="C28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="2"/>
@@ -1541,7 +1555,7 @@
         <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1549,7 +1563,7 @@
         <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1557,7 +1571,7 @@
         <v>9</v>
       </c>
       <c r="C31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1570,7 +1584,7 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D33" t="str">
         <f>CONCATENATE("Insert into TipoFormaConciliacion values(",$A$32,",",B33,",'');")</f>
@@ -1582,7 +1596,7 @@
         <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D34" t="str">
         <f t="shared" ref="D34:D41" si="3">CONCATENATE("Insert into TipoFormaConciliacion values(",$A$32,",",B34,",'');")</f>
@@ -1594,7 +1608,7 @@
         <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D35" t="str">
         <f t="shared" si="3"/>
@@ -1606,7 +1620,7 @@
         <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1614,7 +1628,7 @@
         <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D37" t="str">
         <f t="shared" si="3"/>
@@ -1626,7 +1640,7 @@
         <v>6</v>
       </c>
       <c r="C38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D38" t="str">
         <f t="shared" si="3"/>
@@ -1638,7 +1652,7 @@
         <v>7</v>
       </c>
       <c r="C39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D39" t="str">
         <f t="shared" si="3"/>
@@ -1650,7 +1664,7 @@
         <v>8</v>
       </c>
       <c r="C40" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D40" t="str">
         <f t="shared" si="3"/>
@@ -1662,7 +1676,7 @@
         <v>9</v>
       </c>
       <c r="C41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D41" t="str">
         <f t="shared" si="3"/>
@@ -1670,124 +1684,124 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="5">
+      <c r="A42" s="4">
         <v>5</v>
       </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4">
         <v>1</v>
       </c>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5" t="s">
+      <c r="C43" s="4"/>
+      <c r="D43" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4">
+        <v>2</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D44" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5">
-        <v>2</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4">
         <v>3</v>
       </c>
-      <c r="C45" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
+      <c r="C45" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
-      <c r="B46" s="5">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4">
         <v>4</v>
       </c>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4">
         <v>5</v>
       </c>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5">
+      <c r="A48" s="4"/>
+      <c r="B48" s="4">
         <v>6</v>
       </c>
-      <c r="C48" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
+      <c r="C48" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
-      <c r="B49" s="5">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4">
         <v>7</v>
       </c>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5">
+      <c r="A50" s="4"/>
+      <c r="B50" s="4">
         <v>8</v>
       </c>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="5"/>
-      <c r="B51" s="5">
+      <c r="A51" s="4"/>
+      <c r="B51" s="4">
         <v>9</v>
       </c>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
@@ -1799,7 +1813,7 @@
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -1807,7 +1821,7 @@
         <v>2</v>
       </c>
       <c r="C54" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -1815,7 +1829,7 @@
         <v>3</v>
       </c>
       <c r="C55" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -1823,7 +1837,7 @@
         <v>4</v>
       </c>
       <c r="C56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -1831,7 +1845,7 @@
         <v>5</v>
       </c>
       <c r="C57" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -1839,7 +1853,7 @@
         <v>6</v>
       </c>
       <c r="C58" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -1847,10 +1861,10 @@
         <v>7</v>
       </c>
       <c r="C59" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D59" t="str">
-        <f t="shared" ref="D54:D61" si="4">CONCATENATE("Insert into TipoFormaConciliacion values(",$A$52,",",B59,",'');")</f>
+        <f t="shared" ref="D59:D61" si="4">CONCATENATE("Insert into TipoFormaConciliacion values(",$A$52,",",B59,",'');")</f>
         <v>Insert into TipoFormaConciliacion values(6,7,'');</v>
       </c>
     </row>
@@ -1859,7 +1873,7 @@
         <v>8</v>
       </c>
       <c r="C60" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D60" t="str">
         <f t="shared" si="4"/>
@@ -1871,7 +1885,7 @@
         <v>9</v>
       </c>
       <c r="C61" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D61" t="str">
         <f t="shared" si="4"/>

</xml_diff>